<commit_message>
new dataset (MIDI file monotrack)
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -415,7 +415,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -431,13 +431,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -452,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -462,6 +473,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -796,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A65" sqref="A1:E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -828,118 +848,118 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C2" s="2">
-        <v>-0.48</v>
+        <v>0.37</v>
       </c>
       <c r="D2" s="2">
-        <v>-0.22</v>
+        <v>-0.13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C3" s="2">
-        <v>-0.22</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D3" s="2">
-        <v>0.37</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>127</v>
+        <v>-0.08</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C4" s="2">
-        <v>0.28000000000000003</v>
+        <v>0.2</v>
       </c>
       <c r="D4" s="2">
-        <v>0.42</v>
+        <v>-0.05</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C5" s="2">
-        <v>-0.25</v>
+        <v>0.42</v>
       </c>
       <c r="D5" s="2">
-        <v>0.02</v>
+        <v>-0.18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C6" s="2">
-        <v>0.28999999999999998</v>
+        <v>0.08</v>
       </c>
       <c r="D6" s="2">
-        <v>0.1</v>
+        <v>-0.08</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="C7" s="2">
-        <v>-0.18</v>
+        <v>0.02</v>
       </c>
       <c r="D7" s="2">
-        <v>0.02</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="C8" s="2">
-        <v>0.37</v>
+        <v>0.13</v>
       </c>
       <c r="D8" s="2">
-        <v>-0.13</v>
+        <v>-0.18</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>129</v>
@@ -947,19 +967,19 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="C9" s="2">
-        <v>0.28000000000000003</v>
+        <v>0.03</v>
       </c>
       <c r="D9" s="2">
-        <v>0.67</v>
+        <v>-0.2</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -967,64 +987,64 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="C10" s="2">
-        <v>0.28000000000000003</v>
+        <v>0.47</v>
       </c>
       <c r="D10" s="2">
-        <v>-0.08</v>
-      </c>
-      <c r="E10" s="3" t="s">
+        <v>-0.05</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="C11" s="2">
-        <v>-0.08</v>
+        <v>0.32</v>
       </c>
       <c r="D11" s="2">
-        <v>0.02</v>
+        <v>-0.13</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="C12" s="2">
-        <v>-0.5</v>
+        <v>0.38</v>
       </c>
       <c r="D12" s="2">
-        <v>-0.33</v>
+        <v>-0.32</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="C13" s="2">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D13" s="2">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>129</v>
@@ -1032,19 +1052,19 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="C14" s="2">
-        <v>-0.28000000000000003</v>
+        <v>0.1</v>
       </c>
       <c r="D14" s="2">
-        <v>-0.17</v>
+        <v>-0.33</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1052,13 +1072,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="C15" s="2">
-        <v>0.42</v>
+        <v>0.47</v>
       </c>
       <c r="D15" s="2">
-        <v>-0.18</v>
+        <v>-0.12</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>129</v>
@@ -1066,135 +1086,135 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="C16" s="2">
-        <v>-0.43</v>
+        <v>0.12</v>
       </c>
       <c r="D16" s="2">
-        <v>-0.38</v>
+        <v>-0.32</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>70</v>
+        <v>113</v>
       </c>
       <c r="C17" s="2">
-        <v>-0.47</v>
+        <v>0.25</v>
       </c>
       <c r="D17" s="2">
-        <v>0.1</v>
+        <v>-0.35</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="C18" s="2">
-        <v>0.22</v>
+        <v>0.27</v>
       </c>
       <c r="D18" s="2">
-        <v>0.08</v>
+        <v>-0.3</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="C19" s="2">
-        <v>-0.22</v>
+        <v>0.18</v>
       </c>
       <c r="D19" s="2">
-        <v>0.15</v>
+        <v>-0.02</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="C20" s="2">
-        <v>0.47</v>
+        <v>0.13</v>
       </c>
       <c r="D20" s="2">
-        <v>0.02</v>
+        <v>-0.25</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="C21" s="2">
-        <v>-0.43</v>
+        <v>0.1</v>
       </c>
       <c r="D21" s="2">
-        <v>-0.1</v>
+        <v>-0.05</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C22" s="2">
-        <v>-0.43</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D22" s="2">
-        <v>-7.0000000000000007E-2</v>
+        <v>0.42</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="2" t="s">
-        <v>22</v>
+      <c r="A23" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C23" s="2">
-        <v>0.38</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D23" s="2">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>128</v>
@@ -1202,118 +1222,118 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="C24" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="D25" s="2">
         <v>0.08</v>
       </c>
-      <c r="D24" s="2">
-        <v>-0.08</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="D25" s="2">
-        <v>-7.0000000000000007E-2</v>
-      </c>
       <c r="E25" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C26" s="2">
-        <v>-0.12</v>
+        <v>0.47</v>
       </c>
       <c r="D26" s="2">
-        <v>-0.15</v>
+        <v>0.02</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C27" s="2">
-        <v>-0.23</v>
+        <v>0.38</v>
       </c>
       <c r="D27" s="2">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C28" s="2">
-        <v>-0.38</v>
+        <v>0.25</v>
       </c>
       <c r="D28" s="2">
-        <v>-0.13</v>
+        <v>0.18</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C29" s="2">
-        <v>-0.5</v>
+        <v>0.23</v>
       </c>
       <c r="D29" s="2">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C30" s="2">
-        <v>0.25</v>
+        <v>0.13</v>
       </c>
       <c r="D30" s="2">
-        <v>0.18</v>
+        <v>0.13</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>128</v>
@@ -1321,16 +1341,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C31" s="2">
-        <v>0.23</v>
+        <v>0.1</v>
       </c>
       <c r="D31" s="2">
-        <v>0.05</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>128</v>
@@ -1338,33 +1358,33 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="C32" s="2">
-        <v>-0.18</v>
+        <v>0.17</v>
       </c>
       <c r="D32" s="2">
-        <v>0.42</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="C33" s="2">
-        <v>0.13</v>
+        <v>0.25</v>
       </c>
       <c r="D33" s="2">
-        <v>0.13</v>
+        <v>0.22</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>128</v>
@@ -1372,16 +1392,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="C34" s="2">
-        <v>0.1</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D34" s="2">
-        <v>0.56999999999999995</v>
+        <v>0.02</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>128</v>
@@ -1389,101 +1409,101 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="C35" s="2">
-        <v>-0.5</v>
+        <v>0.03</v>
       </c>
       <c r="D35" s="2">
-        <v>-0.22</v>
+        <v>0.13</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="C36" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="2">
         <v>0.13</v>
       </c>
-      <c r="D36" s="2">
-        <v>-0.18</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C37" s="2">
-        <v>-0.43</v>
-      </c>
       <c r="D37" s="2">
-        <v>-0.2</v>
+        <v>0.48</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="C38" s="2">
-        <v>-0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D38" s="2">
-        <v>-0.32</v>
+        <v>0.22</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="C39" s="2">
-        <v>0.03</v>
+        <v>0.2</v>
       </c>
       <c r="D39" s="2">
-        <v>-0.2</v>
+        <v>0.5</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="2" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="C40" s="2">
-        <v>-0.32</v>
+        <v>-0.22</v>
       </c>
       <c r="D40" s="2">
-        <v>0.25</v>
+        <v>0.37</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>127</v>
@@ -1491,33 +1511,33 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="C41" s="2">
-        <v>0.47</v>
+        <v>-0.25</v>
       </c>
       <c r="D41" s="2">
-        <v>-0.05</v>
+        <v>0.02</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="2" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="C42" s="2">
-        <v>-0.38</v>
+        <v>-0.18</v>
       </c>
       <c r="D42" s="2">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>127</v>
@@ -1525,50 +1545,50 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="C43" s="2">
-        <v>0.32</v>
+        <v>-0.08</v>
       </c>
       <c r="D43" s="2">
-        <v>-0.13</v>
+        <v>0.02</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="2" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="C44" s="2">
-        <v>0.38</v>
+        <v>-0.47</v>
       </c>
       <c r="D44" s="2">
-        <v>-0.32</v>
+        <v>0.1</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="C45" s="2">
-        <v>-0.03</v>
+        <v>-0.22</v>
       </c>
       <c r="D45" s="2">
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>127</v>
@@ -1576,101 +1596,101 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="C46" s="2">
-        <v>0.5</v>
+        <v>-0.23</v>
       </c>
       <c r="D46" s="2">
-        <v>-0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="C47" s="2">
-        <v>0.1</v>
+        <v>-0.5</v>
       </c>
       <c r="D47" s="2">
-        <v>-0.33</v>
+        <v>0.02</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="C48" s="2">
-        <v>0.47</v>
+        <v>-0.18</v>
       </c>
       <c r="D48" s="2">
-        <v>-0.12</v>
+        <v>0.42</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="2" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C49" s="2">
-        <v>-0.12</v>
+        <v>-0.32</v>
       </c>
       <c r="D49" s="2">
-        <v>-0.18</v>
+        <v>0.25</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C50" s="2">
-        <v>0.12</v>
+        <v>-0.38</v>
       </c>
       <c r="D50" s="2">
-        <v>-0.32</v>
+        <v>0.03</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C51" s="2">
-        <v>-0.13</v>
+        <v>-0.03</v>
       </c>
       <c r="D51" s="2">
-        <v>0.32</v>
+        <v>0.12</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>127</v>
@@ -1678,16 +1698,16 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C52" s="2">
-        <v>-0.05</v>
+        <v>-0.13</v>
       </c>
       <c r="D52" s="2">
-        <v>0.02</v>
+        <v>0.32</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>127</v>
@@ -1695,19 +1715,19 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C53" s="2">
-        <v>0.17</v>
+        <v>-0.05</v>
       </c>
       <c r="D53" s="2">
-        <v>0.28000000000000003</v>
+        <v>0.02</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1729,50 +1749,50 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C55" s="2">
-        <v>0.25</v>
+        <v>-0.03</v>
       </c>
       <c r="D55" s="2">
-        <v>0.22</v>
+        <v>0.53</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="2" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>109</v>
+        <v>55</v>
       </c>
       <c r="C56" s="2">
-        <v>0.28000000000000003</v>
+        <v>-0.48</v>
       </c>
       <c r="D56" s="2">
-        <v>0.02</v>
+        <v>-0.22</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="2" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>110</v>
+        <v>65</v>
       </c>
       <c r="C57" s="2">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="D57" s="2">
-        <v>-0.48</v>
+        <v>-0.33</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>126</v>
@@ -1780,67 +1800,67 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="2" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C58" s="2">
-        <v>-0.03</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="D58" s="2">
-        <v>0.53</v>
+        <v>-0.17</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="2" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
       <c r="C59" s="2">
-        <v>0.03</v>
+        <v>-0.43</v>
       </c>
       <c r="D59" s="2">
-        <v>0.13</v>
+        <v>-0.38</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="2" t="s">
-        <v>38</v>
+      <c r="A60" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="C60" s="2">
-        <v>0.25</v>
+        <v>-0.43</v>
       </c>
       <c r="D60" s="2">
-        <v>-0.35</v>
+        <v>-0.1</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="2" t="s">
-        <v>49</v>
+      <c r="A61" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>114</v>
+        <v>75</v>
       </c>
       <c r="C61" s="2">
-        <v>-0.33</v>
+        <v>-0.43</v>
       </c>
       <c r="D61" s="2">
-        <v>-0.33</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>126</v>
@@ -1848,135 +1868,135 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="2" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="C62" s="2">
-        <v>0.27</v>
+        <v>-0.12</v>
       </c>
       <c r="D62" s="2">
-        <v>-0.3</v>
+        <v>-0.15</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="2" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="C63" s="2">
-        <v>0.08</v>
+        <v>-0.38</v>
       </c>
       <c r="D63" s="2">
-        <v>0.18</v>
+        <v>-0.13</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="2" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="C64" s="2">
-        <v>-0.45</v>
+        <v>-0.5</v>
       </c>
       <c r="D64" s="2">
-        <v>-0.37</v>
+        <v>-0.22</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="2" t="s">
-        <v>52</v>
+      <c r="A65" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="C65" s="2">
-        <v>0.18</v>
+        <v>-0.43</v>
       </c>
       <c r="D65" s="2">
-        <v>-0.02</v>
+        <v>-0.2</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C66" s="2">
+        <v>-0.08</v>
+      </c>
+      <c r="D66" s="2">
+        <v>-0.32</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C66" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="D66" s="2">
-        <v>0.48</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="B67" s="2" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="C67" s="2">
-        <v>0.13</v>
+        <v>-0.12</v>
       </c>
       <c r="D67" s="2">
-        <v>-0.25</v>
+        <v>-0.18</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="2" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C68" s="2">
-        <v>0.1</v>
+        <v>-0.25</v>
       </c>
       <c r="D68" s="2">
-        <v>-0.05</v>
+        <v>-0.48</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="2" t="s">
-        <v>32</v>
+      <c r="A69" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C69" s="2">
-        <v>-0.38</v>
+        <v>-0.33</v>
       </c>
       <c r="D69" s="2">
-        <v>-0.22</v>
+        <v>-0.33</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>126</v>
@@ -1984,33 +2004,33 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C70" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>-0.45</v>
       </c>
       <c r="D70" s="2">
-        <v>0.22</v>
+        <v>-0.37</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="2" t="s">
-        <v>54</v>
+      <c r="A71" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C71" s="2">
-        <v>-0.3</v>
+        <v>-0.38</v>
       </c>
       <c r="D71" s="2">
-        <v>-0.27</v>
+        <v>-0.22</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>126</v>
@@ -2018,23 +2038,27 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="2" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C72" s="2">
-        <v>0.2</v>
+        <v>-0.3</v>
       </c>
       <c r="D72" s="2">
-        <v>0.5</v>
+        <v>-0.27</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:E72">
+    <sortCondition ref="E1"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>